<commit_message>
Z calc using log method
</commit_message>
<xml_diff>
--- a/Q3 - 2x2 example.xlsx
+++ b/Q3 - 2x2 example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fl_cl\OneDrive - University College London\Visual Studio 2017\GM_group_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC217D06-21BD-47E6-9736-F163660634B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C13446-32A7-40FE-971C-66D037C607D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,16 +41,10 @@
     <t>pots</t>
   </si>
   <si>
-    <t>b=</t>
-  </si>
-  <si>
     <t>potential</t>
   </si>
   <si>
     <t>Z</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>prob</t>
@@ -70,6 +64,12 @@
   <si>
     <t>state sum</t>
   </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>log(Z)</t>
+  </si>
 </sst>
 </file>
 
@@ -84,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,8 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,56 +428,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -491,47 +499,47 @@
         <f>E2*F2*E3*F3</f>
         <v>54.598150033144229</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <f>SUM(H2:H48)</f>
         <v>199.86497325345624</v>
       </c>
-      <c r="L2">
-        <f>J2/(2^(2*2))</f>
-        <v>12.491560828341015</v>
-      </c>
-      <c r="N2">
+      <c r="K2" s="2">
+        <f>LOG(J2)</f>
+        <v>2.3007366897878248</v>
+      </c>
+      <c r="M2">
         <f>H2/$J$2</f>
         <v>0.2731751799446433</v>
       </c>
-      <c r="O2">
-        <f>SUM(N2:N47)</f>
+      <c r="N2">
+        <f>SUM(M2:M47)</f>
         <v>0.99999999999999978</v>
       </c>
+      <c r="P2">
+        <f>C2</f>
+        <v>0</v>
+      </c>
       <c r="Q2">
-        <f>C2</f>
+        <f>C3</f>
         <v>0</v>
       </c>
       <c r="R2">
-        <f>C3</f>
+        <f>P2+2*Q2</f>
         <v>0</v>
       </c>
       <c r="S2">
-        <f>Q2+2*R2</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <f>SUMIF($R:$R,0,$M:$M)</f>
+        <v>0.38408590099770606</v>
       </c>
       <c r="U2">
-        <f>SUMIF($S:$S,0,$N:$N)</f>
-        <v>0.38408590099770606</v>
-      </c>
-      <c r="V2">
-        <f>SUMIF($S:$S,2,$N:$N)</f>
+        <f>SUMIF($R:$R,2,$M:$M)</f>
         <v>0.11591409900229391</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -546,24 +554,24 @@
         <f>IF(C2=C3,EXP($B$1),1)</f>
         <v>2.7182818284590451</v>
       </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
       <c r="T3">
-        <v>1</v>
+        <f>SUMIF($R:$R,1,$M:$M)</f>
+        <v>0.11591409900229391</v>
       </c>
       <c r="U3">
-        <f>SUMIF($S:$S,1,$N:$N)</f>
-        <v>0.11591409900229391</v>
-      </c>
-      <c r="V3">
-        <f>SUMIF($S:$S,3,$N:$N)</f>
+        <f>SUMIF($R:$R,3,$M:$M)</f>
         <v>0.38408590099770612</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T4">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -585,27 +593,27 @@
         <f>E5*F5*E6*F6</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N5">
+      <c r="M5">
         <f>H5/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P5">
+        <f>C5</f>
+        <v>0</v>
+      </c>
       <c r="Q5">
-        <f>C5</f>
+        <f>C6</f>
         <v>0</v>
       </c>
       <c r="R5">
-        <f>C6</f>
+        <f>P5+2*Q5</f>
         <v>0</v>
       </c>
       <c r="S5">
-        <f>Q5+2*R5</f>
-        <v>0</v>
-      </c>
-      <c r="T5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
@@ -621,7 +629,7 @@
         <v>2.7182818284590451</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -643,24 +651,24 @@
         <f>E8*F8*E9*F9</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N8">
+      <c r="M8">
         <f>H8/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P8">
+        <f>C8</f>
+        <v>1</v>
+      </c>
       <c r="Q8">
-        <f>C8</f>
-        <v>1</v>
+        <f>C9</f>
+        <v>0</v>
       </c>
       <c r="R8">
-        <f>C9</f>
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <f>Q8+2*R8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+        <f>P8+2*Q8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>0</v>
       </c>
@@ -676,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>A8+1</f>
         <v>3</v>
@@ -699,24 +707,24 @@
         <f>E11*F11*E12*F12</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N11">
+      <c r="M11">
         <f>H11/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P11">
+        <f>C11</f>
+        <v>1</v>
+      </c>
       <c r="Q11">
-        <f>C11</f>
-        <v>1</v>
+        <f>C12</f>
+        <v>0</v>
       </c>
       <c r="R11">
-        <f>C12</f>
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <f>Q11+2*R11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+        <f>P11+2*Q11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0</v>
       </c>
@@ -732,16 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="J13">
-        <v>6</v>
-      </c>
-      <c r="K13">
-        <f>EXP(J13)</f>
-        <v>403.42879349273511</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>A11+1</f>
         <v>4</v>
@@ -764,24 +763,24 @@
         <f>E14*F14*E15*F15</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N14">
+      <c r="M14">
         <f>H14/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P14">
+        <f>C14</f>
+        <v>0</v>
+      </c>
       <c r="Q14">
-        <f>C14</f>
+        <f>C15</f>
         <v>0</v>
       </c>
       <c r="R14">
-        <f>C15</f>
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <f>Q14+2*R14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+        <f>P14+2*Q14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1</v>
       </c>
@@ -797,7 +796,7 @@
         <v>2.7182818284590451</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <f>A14+1</f>
         <v>5</v>
@@ -820,24 +819,24 @@
         <f>E17*F17*E18*F18</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N17">
+      <c r="M17">
         <f>H17/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P17">
+        <f>C17</f>
+        <v>0</v>
+      </c>
       <c r="Q17">
-        <f>C17</f>
+        <f>C18</f>
         <v>0</v>
       </c>
       <c r="R17">
-        <f>C18</f>
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <f>Q17+2*R17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+        <f>P17+2*Q17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>1</v>
       </c>
@@ -853,7 +852,7 @@
         <v>2.7182818284590451</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <f>A17+1</f>
         <v>6</v>
@@ -876,24 +875,24 @@
         <f>E20*F20*E21*F21</f>
         <v>1</v>
       </c>
-      <c r="N20">
+      <c r="M20">
         <f>H20/$J$2</f>
         <v>5.0033779492310668E-3</v>
       </c>
+      <c r="P20">
+        <f>C20</f>
+        <v>1</v>
+      </c>
       <c r="Q20">
-        <f>C20</f>
-        <v>1</v>
+        <f>C21</f>
+        <v>0</v>
       </c>
       <c r="R20">
-        <f>C21</f>
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <f>Q20+2*R20</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+        <f>P20+2*Q20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>1</v>
       </c>
@@ -909,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <f>A20+1</f>
         <v>7</v>
@@ -932,24 +931,24 @@
         <f>E23*F23*E24*F24</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N23">
+      <c r="M23">
         <f>H23/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P23">
+        <f>C23</f>
+        <v>1</v>
+      </c>
       <c r="Q23">
-        <f>C23</f>
-        <v>1</v>
+        <f>C24</f>
+        <v>0</v>
       </c>
       <c r="R23">
-        <f>C24</f>
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <f>Q23+2*R23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+        <f>P23+2*Q23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1</v>
       </c>
@@ -965,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <f>A23+1</f>
         <v>8</v>
@@ -988,24 +987,24 @@
         <f>E26*F26*E27*F27</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N26">
+      <c r="M26">
         <f>H26/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P26">
+        <f>C26</f>
+        <v>0</v>
+      </c>
       <c r="Q26">
-        <f>C26</f>
-        <v>0</v>
+        <f>C27</f>
+        <v>1</v>
       </c>
       <c r="R26">
-        <f>C27</f>
-        <v>1</v>
-      </c>
-      <c r="S26">
-        <f>Q26+2*R26</f>
+        <f>P26+2*Q26</f>
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>0</v>
       </c>
@@ -1021,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <f>A26+1</f>
         <v>9</v>
@@ -1044,24 +1043,24 @@
         <f>E29*F29*E30*F30</f>
         <v>1</v>
       </c>
-      <c r="N29">
+      <c r="M29">
         <f>H29/$J$2</f>
         <v>5.0033779492310668E-3</v>
       </c>
+      <c r="P29">
+        <f>C29</f>
+        <v>0</v>
+      </c>
       <c r="Q29">
-        <f>C29</f>
-        <v>0</v>
+        <f>C30</f>
+        <v>1</v>
       </c>
       <c r="R29">
-        <f>C30</f>
-        <v>1</v>
-      </c>
-      <c r="S29">
-        <f>Q29+2*R29</f>
+        <f>P29+2*Q29</f>
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>0</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <f>A29+1</f>
         <v>10</v>
@@ -1100,24 +1099,24 @@
         <f>E32*F32*E33*F33</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N32">
+      <c r="M32">
         <f>H32/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P32">
+        <f>C32</f>
+        <v>1</v>
+      </c>
       <c r="Q32">
-        <f>C32</f>
+        <f>C33</f>
         <v>1</v>
       </c>
       <c r="R32">
-        <f>C33</f>
-        <v>1</v>
-      </c>
-      <c r="S32">
-        <f>Q32+2*R32</f>
+        <f>P32+2*Q32</f>
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>0</v>
       </c>
@@ -1133,7 +1132,7 @@
         <v>2.7182818284590451</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>A32+1</f>
         <v>11</v>
@@ -1156,24 +1155,24 @@
         <f>E35*F35*E36*F36</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N35">
+      <c r="M35">
         <f>H35/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P35">
+        <f>C35</f>
+        <v>1</v>
+      </c>
       <c r="Q35">
-        <f>C35</f>
+        <f>C36</f>
         <v>1</v>
       </c>
       <c r="R35">
-        <f>C36</f>
-        <v>1</v>
-      </c>
-      <c r="S35">
-        <f>Q35+2*R35</f>
+        <f>P35+2*Q35</f>
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>0</v>
       </c>
@@ -1189,7 +1188,7 @@
         <v>2.7182818284590451</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38">
         <f>A35+1</f>
         <v>12</v>
@@ -1212,24 +1211,24 @@
         <f>E38*F38*E39*F39</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N38">
+      <c r="M38">
         <f>H38/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P38">
+        <f>C38</f>
+        <v>0</v>
+      </c>
       <c r="Q38">
-        <f>C38</f>
-        <v>0</v>
+        <f>C39</f>
+        <v>1</v>
       </c>
       <c r="R38">
-        <f>C39</f>
-        <v>1</v>
-      </c>
-      <c r="S38">
-        <f>Q38+2*R38</f>
+        <f>P38+2*Q38</f>
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>1</v>
       </c>
@@ -1245,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>A38+1</f>
         <v>13</v>
@@ -1268,24 +1267,24 @@
         <f>E41*F41*E42*F42</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N41">
+      <c r="M41">
         <f>H41/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P41">
+        <f>C41</f>
+        <v>0</v>
+      </c>
       <c r="Q41">
-        <f>C41</f>
-        <v>0</v>
+        <f>C42</f>
+        <v>1</v>
       </c>
       <c r="R41">
-        <f>C42</f>
-        <v>1</v>
-      </c>
-      <c r="S41">
-        <f>Q41+2*R41</f>
+        <f>P41+2*Q41</f>
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>1</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44">
         <f>A41+1</f>
         <v>14</v>
@@ -1324,24 +1323,24 @@
         <f>E44*F44*E45*F45</f>
         <v>7.3890560989306495</v>
       </c>
-      <c r="N44">
+      <c r="M44">
         <f>H44/$J$2</f>
         <v>3.6970240351020943E-2</v>
       </c>
+      <c r="P44">
+        <f>C44</f>
+        <v>1</v>
+      </c>
       <c r="Q44">
-        <f>C44</f>
+        <f>C45</f>
         <v>1</v>
       </c>
       <c r="R44">
-        <f>C45</f>
-        <v>1</v>
-      </c>
-      <c r="S44">
-        <f>Q44+2*R44</f>
+        <f>P44+2*Q44</f>
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>1</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>2.7182818284590451</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47">
         <f>A44+1</f>
         <v>15</v>
@@ -1380,24 +1379,24 @@
         <f>E47*F47*E48*F48</f>
         <v>54.598150033144229</v>
       </c>
-      <c r="N47">
+      <c r="M47">
         <f>H47/$J$2</f>
         <v>0.2731751799446433</v>
       </c>
+      <c r="P47">
+        <f>C47</f>
+        <v>1</v>
+      </c>
       <c r="Q47">
-        <f>C47</f>
+        <f>C48</f>
         <v>1</v>
       </c>
       <c r="R47">
-        <f>C48</f>
-        <v>1</v>
-      </c>
-      <c r="S47">
-        <f>Q47+2*R47</f>
+        <f>P47+2*Q47</f>
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>1</v>
       </c>

</xml_diff>